<commit_message>
Update ReadMe for general commodity and clarity.
</commit_message>
<xml_diff>
--- a/parameters/DJ/ammonia/country_parameters.xlsx
+++ b/parameters/DJ/ammonia/country_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/hert5576_ox_ac_uk/Documents/CCG/GEOH2/ETH Hydrogen Collaboration/Ammonia model runs/Inputs and results v3 2023-10-18/GEONH3/Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hert5576\PycharmProjects\GeoH2\parameters\DJ\ammonia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{047B2753-744E-4748-BCC3-0DA81507078E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A764A543-B473-4FD8-B7AA-851B913C76E3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E748F03-F7B2-4D22-A8CC-5CF572A1D69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{60BD1E41-9A81-F547-A629-52DD9269BE2D}"/>
+    <workbookView xWindow="1837" yWindow="1837" windowWidth="16201" windowHeight="9428" xr2:uid="{60BD1E41-9A81-F547-A629-52DD9269BE2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Country</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Djibouti</t>
-  </si>
-  <si>
-    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -129,9 +126,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -169,7 +166,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -275,7 +272,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -417,7 +414,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -425,27 +422,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A655327-FB0F-D040-A870-A9F18A82B881}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="23.796875" customWidth="1"/>
-    <col min="2" max="2" width="24.69921875" customWidth="1"/>
-    <col min="3" max="3" width="24.296875" customWidth="1"/>
-    <col min="4" max="4" width="19.69921875" customWidth="1"/>
+    <col min="1" max="1" width="23.8125" customWidth="1"/>
+    <col min="2" max="2" width="24.6875" customWidth="1"/>
+    <col min="3" max="3" width="24.3125" customWidth="1"/>
+    <col min="4" max="4" width="19.6875" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="26.19921875" customWidth="1"/>
-    <col min="7" max="7" width="19.796875" customWidth="1"/>
-    <col min="8" max="8" width="20.19921875" customWidth="1"/>
-    <col min="9" max="9" width="18.19921875" customWidth="1"/>
+    <col min="6" max="6" width="26.1875" customWidth="1"/>
+    <col min="7" max="7" width="19.8125" customWidth="1"/>
+    <col min="8" max="8" width="20.1875" customWidth="1"/>
+    <col min="9" max="9" width="18.1875" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,7 +477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -512,41 +509,6 @@
         <v>5.6800000000000003E-2</v>
       </c>
       <c r="K2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>0.2366</v>
-      </c>
-      <c r="C3">
-        <v>0.02</v>
-      </c>
-      <c r="D3">
-        <v>9.6289000000000013E-2</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="F3">
-        <v>9.6289000000000013E-2</v>
-      </c>
-      <c r="G3">
-        <v>20</v>
-      </c>
-      <c r="H3">
-        <v>9.6289000000000013E-2</v>
-      </c>
-      <c r="I3">
-        <v>20</v>
-      </c>
-      <c r="J3">
-        <v>5.6800000000000003E-2</v>
-      </c>
-      <c r="K3">
         <v>50</v>
       </c>
     </row>

</xml_diff>